<commit_message>
Se muestran solo las estaciones que se visitan
</commit_message>
<xml_diff>
--- a/datos_salida/Recorrido_Estaciones_Unidades.xlsx
+++ b/datos_salida/Recorrido_Estaciones_Unidades.xlsx
@@ -7,10 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Turno 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Turno 2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Turno 3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Turno 4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Vuelta 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Vuelta 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Vuelta 3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14598,4730 +14597,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K96"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Placa de tracto</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Empresa</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Capacidad total</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t># Compartimentos</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Orden de llegada</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Destinatario</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t># Distrito</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Estación</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Dirección</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Grupo</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ACG-766</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>10400</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>P294</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>BARRANCA</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>E/S SAN JOSÉ</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Av. Panamericana Nte. 928, Barranca 15169</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ACG-766</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>10400</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>P118</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>BARRANCA</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>E/S BARRANCA</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Pje. Callao 104, Barranca 15169</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ACG-766</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>10400</v>
-      </c>
-      <c r="E4" t="n">
-        <v>5</v>
-      </c>
-      <c r="F4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>P113</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>HUARAL</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>E/S HUARALINO</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Chancay 351, Huaral 15202</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ACG-766</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>10400</v>
-      </c>
-      <c r="E5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>P135</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>ATE</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>E/S ATE 1</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Tomas Alva Edison 160, Lima 15022</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ACG-766</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>10400</v>
-      </c>
-      <c r="E6" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>5</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>P292</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>LURIN</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>E/S SAN CARLOS</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>P4H3+35F, Lurín 15823</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>AWJ-767</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>CORPORACIÓN ENRIQUE &amp; JANIS</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E7" t="n">
-        <v>7</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>P113</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>HUARAL</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>E/S HUARALINO</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Chancay 351, Huaral 15202</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>AWJ-767</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>CORPORACIÓN ENRIQUE &amp; JANIS</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E8" t="n">
-        <v>7</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>P135</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>ATE</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>E/S ATE 1</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Tomas Alva Edison 160, Lima 15022</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>AWJ-767</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>CORPORACIÓN ENRIQUE &amp; JANIS</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E9" t="n">
-        <v>7</v>
-      </c>
-      <c r="F9" t="n">
-        <v>3</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>P292</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>LURIN</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>E/S SAN CARLOS</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>P4H3+35F, Lurín 15823</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>AWJ-767</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>CORPORACIÓN ENRIQUE &amp; JANIS</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E10" t="n">
-        <v>7</v>
-      </c>
-      <c r="F10" t="n">
-        <v>4</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>P226</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>MAGDALENA DEL MAR</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>E/S FLORA TRISTAN</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Av Javier Prado Oeste 2504, Magdalena del Mar 15076</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>BJL-708</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>INVERSIONES JULIO III</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E11" t="n">
-        <v>9</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>P292</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>LURIN</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>E/S SAN CARLOS</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>P4H3+35F, Lurín 15823</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>BJL-708</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>INVERSIONES JULIO III</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E12" t="n">
-        <v>9</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>P226</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>MAGDALENA DEL MAR</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>E/S FLORA TRISTAN</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Av Javier Prado Oeste 2504, Magdalena del Mar 15076</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>AYR-771</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E13" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>P132</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>SAN MARTÍN DE PORRES</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>E/S TOMÁS VALLE</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Av. Tomas Valle 846, San Martín de Porres 15302</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>AYR-771</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E14" t="n">
-        <v>3</v>
-      </c>
-      <c r="F14" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>P317</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>CERCADO DE LIMA</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>E/S TINGO MARIA</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Avenida Tingo Maria Chacra Rios Sur 1711, Cercado de Lima 15083</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>AYR-771</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E15" t="n">
-        <v>3</v>
-      </c>
-      <c r="F15" t="n">
-        <v>3</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>P191</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>CALLAO</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>E/S MARCO POLO</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Av. Marco Polo, Callao 07021</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>AYR-771</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E16" t="n">
-        <v>3</v>
-      </c>
-      <c r="F16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>P160</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>PUEBLO LIBRE</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>E/S BOLÍVAR</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>WWHP+649, Pueblo Libre 15084</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>AYR-771</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E17" t="n">
-        <v>3</v>
-      </c>
-      <c r="F17" t="n">
-        <v>5</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>P226</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>MAGDALENA DEL MAR</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>E/S FLORA TRISTAN</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Av Javier Prado Oeste 2504, Magdalena del Mar 15076</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>BED-794</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" t="n">
-        <v>1</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>P132</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>SAN MARTÍN DE PORRES</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>E/S TOMÁS VALLE</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Av. Tomas Valle 846, San Martín de Porres 15302</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>BED-794</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>P317</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>CERCADO DE LIMA</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>E/S TINGO MARIA</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>Avenida Tingo Maria Chacra Rios Sur 1711, Cercado de Lima 15083</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>BED-794</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" t="n">
-        <v>3</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>P160</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>PUEBLO LIBRE</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>E/S BOLÍVAR</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>WWHP+649, Pueblo Libre 15084</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>BED-794</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" t="n">
-        <v>4</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>P277</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>LA PERLA</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>E/S PERLA</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>La Paz 2370, La Perla 07016</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>AXY-949</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>TRANSPORTES GENERALES J&amp;F S.A.C</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E22" t="n">
-        <v>3</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>P132</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>SAN MARTÍN DE PORRES</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>E/S TOMÁS VALLE</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Av. Tomas Valle 846, San Martín de Porres 15302</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>AXY-949</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>TRANSPORTES GENERALES J&amp;F S.A.C</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F23" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>P191</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>CALLAO</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>E/S MARCO POLO</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>Av. Marco Polo, Callao 07021</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>AXY-949</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>TRANSPORTES GENERALES J&amp;F S.A.C</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E24" t="n">
-        <v>3</v>
-      </c>
-      <c r="F24" t="n">
-        <v>3</v>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>P160</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>PUEBLO LIBRE</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>E/S BOLÍVAR</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>WWHP+649, Pueblo Libre 15084</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>AXY-949</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>TRANSPORTES GENERALES J&amp;F S.A.C</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E25" t="n">
-        <v>3</v>
-      </c>
-      <c r="F25" t="n">
-        <v>4</v>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>P277</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>LA PERLA</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>E/S PERLA</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>La Paz 2370, La Perla 07016</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>AXY-949</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>TRANSPORTES GENERALES J&amp;F S.A.C</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E26" t="n">
-        <v>3</v>
-      </c>
-      <c r="F26" t="n">
-        <v>5</v>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>P102</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>LA VICTORIA</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>E/S 28 DE JULIO</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>Avenida 28 de Julio 2200, La Victoria 15018</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>AXY-949</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>TRANSPORTES GENERALES J&amp;F S.A.C</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F27" t="n">
-        <v>6</v>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>P157</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>SAN BORJA</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>E/S PRINCIPAL</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>Jr. Ernesto Rutherford 103, Distrito de Lima 15036</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>D5D-868</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>HERMELINDA HUATAY MANTILLA</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E28" t="n">
-        <v>6</v>
-      </c>
-      <c r="F28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>P277</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>LA PERLA</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>E/S PERLA</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>La Paz 2370, La Perla 07016</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>D5D-868</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>HERMELINDA HUATAY MANTILLA</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E29" t="n">
-        <v>6</v>
-      </c>
-      <c r="F29" t="n">
-        <v>2</v>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>P102</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>LA VICTORIA</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>E/S 28 DE JULIO</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>Avenida 28 de Julio 2200, La Victoria 15018</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>D5D-868</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>HERMELINDA HUATAY MANTILLA</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E30" t="n">
-        <v>6</v>
-      </c>
-      <c r="F30" t="n">
-        <v>3</v>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>P152</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>SAN BORJA</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>E/S NAVAL</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>Av. San Luis 2480, San Borja 15037</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>D5D-868</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>HERMELINDA HUATAY MANTILLA</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E31" t="n">
-        <v>6</v>
-      </c>
-      <c r="F31" t="n">
-        <v>4</v>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>P269</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>ÑAÑA</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>E/S ÑAÑA</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>Carr. Central 912, Chaclacayo 15476</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>AYX-789</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>JWENVERT TRANSPORTES</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E32" t="n">
-        <v>8</v>
-      </c>
-      <c r="F32" t="n">
-        <v>1</v>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>P269</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>ÑAÑA</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>E/S ÑAÑA</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>Carr. Central 912, Chaclacayo 15476</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>AYX-789</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>JWENVERT TRANSPORTES</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E33" t="n">
-        <v>8</v>
-      </c>
-      <c r="F33" t="n">
-        <v>2</v>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>P157</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>SAN BORJA</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>E/S PRINCIPAL</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Jr. Ernesto Rutherford 103, Distrito de Lima 15036</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>AYX-789</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>JWENVERT TRANSPORTES</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E34" t="n">
-        <v>8</v>
-      </c>
-      <c r="F34" t="n">
-        <v>3</v>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>P180</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>VILLA EL SALVADOR</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>E/S VILLA EL SALVADOR</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>R24P+P5X, Villa EL Salvador 15842</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>AYX-789</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>JWENVERT TRANSPORTES</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E35" t="n">
-        <v>8</v>
-      </c>
-      <c r="F35" t="n">
-        <v>4</v>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>P289</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>LINCE</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>E/S SALAVERRY 1</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>Av. César Canevaro 1598, Lince 15073</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>BBF-813</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>CORPORACIÓN ENRIQUE &amp; JANIS</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E36" t="n">
-        <v>7</v>
-      </c>
-      <c r="F36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>P296</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>SAN LUIS</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>E/S SAN LUIS 1</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>Av. Nicolás Ayllón 1340, San Luis 15019</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>BBF-813</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>CORPORACIÓN ENRIQUE &amp; JANIS</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E37" t="n">
-        <v>7</v>
-      </c>
-      <c r="F37" t="n">
-        <v>2</v>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>P157</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>SAN BORJA</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>E/S PRINCIPAL</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>Jr. Ernesto Rutherford 103, Distrito de Lima 15036</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>BBF-813</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>CORPORACIÓN ENRIQUE &amp; JANIS</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E38" t="n">
-        <v>7</v>
-      </c>
-      <c r="F38" t="n">
-        <v>3</v>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>P162</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>SANTIAGO DE SURCO</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>E/S TOMÁS MARSANO</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>Av Tomás Marsano 4080, Santiago de Surco 15039</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>BBF-813</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>CORPORACIÓN ENRIQUE &amp; JANIS</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E39" t="n">
-        <v>7</v>
-      </c>
-      <c r="F39" t="n">
-        <v>4</v>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>P180</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>VILLA EL SALVADOR</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>E/S VILLA EL SALVADOR</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>R24P+P5X, Villa EL Salvador 15842</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>F3Y-722</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E40" t="n">
-        <v>8</v>
-      </c>
-      <c r="F40" t="n">
-        <v>1</v>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>P325</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>SANTIAGO DE SURCO</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>E/S VALLE HERMOSO</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>V2RF+334, Santiago de Surco 15023</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>F3Y-722</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E41" t="n">
-        <v>8</v>
-      </c>
-      <c r="F41" t="n">
-        <v>2</v>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>P296</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>SAN LUIS</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>E/S SAN LUIS 1</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>Av. Nicolás Ayllón 1340, San Luis 15019</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>F3Y-722</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E42" t="n">
-        <v>8</v>
-      </c>
-      <c r="F42" t="n">
-        <v>3</v>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>P289</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>LINCE</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>E/S SALAVERRY 1</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>Av. César Canevaro 1598, Lince 15073</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>ADY-911</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E43" t="n">
-        <v>6</v>
-      </c>
-      <c r="F43" t="n">
-        <v>1</v>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>P175</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>MAGDALENA DEL MAR</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>E/S SALAVERRY 2</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>Jirón Salaverry 480, Magdalena del Mar 15086</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>ADY-911</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E44" t="n">
-        <v>6</v>
-      </c>
-      <c r="F44" t="n">
-        <v>2</v>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>P289</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>LINCE</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>E/S SALAVERRY 1</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>Av. César Canevaro 1598, Lince 15073</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>ADY-911</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E45" t="n">
-        <v>6</v>
-      </c>
-      <c r="F45" t="n">
-        <v>3</v>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>P325</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>SANTIAGO DE SURCO</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>E/S VALLE HERMOSO</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>V2RF+334, Santiago de Surco 15023</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>C5V-914</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E46" t="n">
-        <v>6</v>
-      </c>
-      <c r="F46" t="n">
-        <v>1</v>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>P126</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>ATE</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>E/S ATE 2</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>Residencial Portales de Pariachi Mz S1 lote 36, Ate 15476</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>C5V-914</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E47" t="n">
-        <v>6</v>
-      </c>
-      <c r="F47" t="n">
-        <v>2</v>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>P175</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>MAGDALENA DEL MAR</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>E/S SALAVERRY 2</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>Jirón Salaverry 480, Magdalena del Mar 15086</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>C5V-914</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E48" t="n">
-        <v>6</v>
-      </c>
-      <c r="F48" t="n">
-        <v>3</v>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>P255</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>CANTO GRANDE</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>E/S LURIGANCHO</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Av. Lurigancho 1175, San Juan de Lurigancho 15427</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>C5V-914</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E49" t="n">
-        <v>6</v>
-      </c>
-      <c r="F49" t="n">
-        <v>4</v>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>P325</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>SANTIAGO DE SURCO</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>E/S VALLE HERMOSO</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>V2RF+334, Santiago de Surco 15023</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>C5V-914</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D50" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E50" t="n">
-        <v>6</v>
-      </c>
-      <c r="F50" t="n">
-        <v>5</v>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>P275</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>LURIN</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>E/S PANSUR</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>Km, Antigua Panamericana Sur 30, Lurín</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>AYR-9452</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D51" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E51" t="n">
-        <v>1</v>
-      </c>
-      <c r="F51" t="n">
-        <v>1</v>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>P175</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>MAGDALENA DEL MAR</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>E/S SALAVERRY 2</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>Jirón Salaverry 480, Magdalena del Mar 15086</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>AYR-9452</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E52" t="n">
-        <v>1</v>
-      </c>
-      <c r="F52" t="n">
-        <v>2</v>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>P211</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>CERCADO DE LIMA</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>E/S DUEÑAS</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>Av. Argentina 629, Cercado de Lima 15081</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>AYR-9452</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D53" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E53" t="n">
-        <v>1</v>
-      </c>
-      <c r="F53" t="n">
-        <v>3</v>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>P101</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>VILLA EL SALVADOR</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>E/S MIGUEL ANGEL</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>Av. Lima 2000, Villa María del Triunfo 15816</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>AYR-9452</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D54" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E54" t="n">
-        <v>1</v>
-      </c>
-      <c r="F54" t="n">
-        <v>4</v>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>P126</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>ATE</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>E/S ATE 2</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>Residencial Portales de Pariachi Mz S1 lote 36, Ate 15476</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>APM-857</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>UL&amp;PH INVERSIONES SAC</t>
-        </is>
-      </c>
-      <c r="D55" t="n">
-        <v>7600</v>
-      </c>
-      <c r="E55" t="n">
-        <v>8</v>
-      </c>
-      <c r="F55" t="n">
-        <v>1</v>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>P283</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>CALLAO</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>E/S QUILCA</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>Av. Quilca 531, San Martín de Porres 15106</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>APM-857</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>UL&amp;PH INVERSIONES SAC</t>
-        </is>
-      </c>
-      <c r="D56" t="n">
-        <v>7600</v>
-      </c>
-      <c r="E56" t="n">
-        <v>8</v>
-      </c>
-      <c r="F56" t="n">
-        <v>2</v>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>P324</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>LA MOLINA</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>E/S UNIVERSIDAD</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>Av. La Universidad 22, La Molina 15026</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>APM-857</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>UL&amp;PH INVERSIONES SAC</t>
-        </is>
-      </c>
-      <c r="D57" t="n">
-        <v>7600</v>
-      </c>
-      <c r="E57" t="n">
-        <v>8</v>
-      </c>
-      <c r="F57" t="n">
-        <v>3</v>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>P175</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>MAGDALENA DEL MAR</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>E/S SALAVERRY 2</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>Jirón Salaverry 480, Magdalena del Mar 15086</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>APM-857</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>UL&amp;PH INVERSIONES SAC</t>
-        </is>
-      </c>
-      <c r="D58" t="n">
-        <v>7600</v>
-      </c>
-      <c r="E58" t="n">
-        <v>8</v>
-      </c>
-      <c r="F58" t="n">
-        <v>4</v>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>P265</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>LA MOLINA</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>E/S MONTERRICO</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>Av. la Molina 580, La Molina 15023</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>APM-857</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>UL&amp;PH INVERSIONES SAC</t>
-        </is>
-      </c>
-      <c r="D59" t="n">
-        <v>7600</v>
-      </c>
-      <c r="E59" t="n">
-        <v>8</v>
-      </c>
-      <c r="F59" t="n">
-        <v>5</v>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>P101</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>VILLA EL SALVADOR</t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>E/S MIGUEL ANGEL</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>Av. Lima 2000, Villa María del Triunfo 15816</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>B7K-982</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D60" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E60" t="n">
-        <v>8</v>
-      </c>
-      <c r="F60" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>P283</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>CALLAO</t>
-        </is>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>E/S QUILCA</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>Av. Quilca 531, San Martín de Porres 15106</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>B7K-982</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D61" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E61" t="n">
-        <v>8</v>
-      </c>
-      <c r="F61" t="n">
-        <v>2</v>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>P255</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>CANTO GRANDE</t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>E/S LURIGANCHO</t>
-        </is>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>Av. Lurigancho 1175, San Juan de Lurigancho 15427</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>B7K-982</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D62" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E62" t="n">
-        <v>8</v>
-      </c>
-      <c r="F62" t="n">
-        <v>3</v>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>P371</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>LA VICTORIA</t>
-        </is>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>E/S LA VICTORIA</t>
-        </is>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>Av. Isabel la Católica 77, La Victoria 15033</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>B7K-982</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D63" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E63" t="n">
-        <v>8</v>
-      </c>
-      <c r="F63" t="n">
-        <v>4</v>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>P270</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>MIRAFLORES</t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>E/S ORRANTIA</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>Av. del Ejército 965, Magdalena del Mar 15076</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>B7K-982</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>TRANSPORTES TESA</t>
-        </is>
-      </c>
-      <c r="D64" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E64" t="n">
-        <v>8</v>
-      </c>
-      <c r="F64" t="n">
-        <v>5</v>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>P181</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>PUNTA HERMOSA</t>
-        </is>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>E/S PUNTA HERMOSA</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>Carr. Panamericana Sur, 1S, Lima</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>ANW-916</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>UL&amp;PH INVERSIONES SAC</t>
-        </is>
-      </c>
-      <c r="D65" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E65" t="n">
-        <v>8</v>
-      </c>
-      <c r="F65" t="n">
-        <v>1</v>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>P270</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>MIRAFLORES</t>
-        </is>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>E/S ORRANTIA</t>
-        </is>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>Av. del Ejército 965, Magdalena del Mar 15076</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>ANW-916</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>UL&amp;PH INVERSIONES SAC</t>
-        </is>
-      </c>
-      <c r="D66" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E66" t="n">
-        <v>8</v>
-      </c>
-      <c r="F66" t="n">
-        <v>2</v>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>P183</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>SURQUILLO</t>
-        </is>
-      </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>E/S ANGAMOS</t>
-        </is>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>Av. Angamos 1401, Surquillo 15048</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>ANW-916</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>UL&amp;PH INVERSIONES SAC</t>
-        </is>
-      </c>
-      <c r="D67" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E67" t="n">
-        <v>8</v>
-      </c>
-      <c r="F67" t="n">
-        <v>3</v>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>P185</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>SANTIAGO DE SURCO</t>
-        </is>
-      </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>E/S JORGE CHÁVEZ</t>
-        </is>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>VX3Q+784, Santiago de Surco 15049</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>ANW-916</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>UL&amp;PH INVERSIONES SAC</t>
-        </is>
-      </c>
-      <c r="D68" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E68" t="n">
-        <v>8</v>
-      </c>
-      <c r="F68" t="n">
-        <v>4</v>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>P371</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>LA VICTORIA</t>
-        </is>
-      </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>E/S LA VICTORIA</t>
-        </is>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>Av. Isabel la Católica 77, La Victoria 15033</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>ANW-916</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>UL&amp;PH INVERSIONES SAC</t>
-        </is>
-      </c>
-      <c r="D69" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E69" t="n">
-        <v>8</v>
-      </c>
-      <c r="F69" t="n">
-        <v>5</v>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>P324</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>LA MOLINA</t>
-        </is>
-      </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>E/S UNIVERSIDAD</t>
-        </is>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>Av. La Universidad 22, La Molina 15026</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>BAC-761</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D70" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E70" t="n">
-        <v>7</v>
-      </c>
-      <c r="F70" t="n">
-        <v>1</v>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>P181</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>PUNTA HERMOSA</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>E/S PUNTA HERMOSA</t>
-        </is>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>Carr. Panamericana Sur, 1S, Lima</t>
-        </is>
-      </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>BAC-761</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D71" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E71" t="n">
-        <v>7</v>
-      </c>
-      <c r="F71" t="n">
-        <v>2</v>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>P185</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>SANTIAGO DE SURCO</t>
-        </is>
-      </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>E/S JORGE CHÁVEZ</t>
-        </is>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>VX3Q+784, Santiago de Surco 15049</t>
-        </is>
-      </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>BAC-761</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D72" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E72" t="n">
-        <v>7</v>
-      </c>
-      <c r="F72" t="n">
-        <v>3</v>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>P266</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>SANTIAGO DE SURCO</t>
-        </is>
-      </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>E/S MONTREAL</t>
-        </is>
-      </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>Av. Caminos del Inca 2017, Santiago de Surco 15039</t>
-        </is>
-      </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>BAC-761</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D73" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E73" t="n">
-        <v>7</v>
-      </c>
-      <c r="F73" t="n">
-        <v>4</v>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>P270</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>MIRAFLORES</t>
-        </is>
-      </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>E/S ORRANTIA</t>
-        </is>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>Av. del Ejército 965, Magdalena del Mar 15076</t>
-        </is>
-      </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>BAC-761</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>LOGISTIC TRANSPORT PERU SAC</t>
-        </is>
-      </c>
-      <c r="D74" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E74" t="n">
-        <v>7</v>
-      </c>
-      <c r="F74" t="n">
-        <v>5</v>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>P183</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>SURQUILLO</t>
-        </is>
-      </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>E/S ANGAMOS</t>
-        </is>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>Av. Angamos 1401, Surquillo 15048</t>
-        </is>
-      </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>AYR-9451</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D75" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E75" t="n">
-        <v>8</v>
-      </c>
-      <c r="F75" t="n">
-        <v>1</v>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>P185</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>SANTIAGO DE SURCO</t>
-        </is>
-      </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>E/S JORGE CHÁVEZ</t>
-        </is>
-      </c>
-      <c r="J75" t="inlineStr">
-        <is>
-          <t>VX3Q+784, Santiago de Surco 15049</t>
-        </is>
-      </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>AYR-9451</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D76" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E76" t="n">
-        <v>8</v>
-      </c>
-      <c r="F76" t="n">
-        <v>2</v>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>P266</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>SANTIAGO DE SURCO</t>
-        </is>
-      </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>E/S MONTREAL</t>
-        </is>
-      </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>Av. Caminos del Inca 2017, Santiago de Surco 15039</t>
-        </is>
-      </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>AYR-9451</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D77" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E77" t="n">
-        <v>8</v>
-      </c>
-      <c r="F77" t="n">
-        <v>3</v>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>P167</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>MIRAFLORES</t>
-        </is>
-      </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>E/S MIRAFLORES</t>
-        </is>
-      </c>
-      <c r="J77" t="inlineStr">
-        <is>
-          <t>VXGG+H2W, Lima 15074</t>
-        </is>
-      </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>AYR-9451</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D78" t="n">
-        <v>7500</v>
-      </c>
-      <c r="E78" t="n">
-        <v>8</v>
-      </c>
-      <c r="F78" t="n">
-        <v>4</v>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>P327</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>ZARATE</t>
-        </is>
-      </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>E/S ZARATE</t>
-        </is>
-      </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>Av. Malecón Checa, San Juan de Lurigancho 15401</t>
-        </is>
-      </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>ANC-872</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>TRANSPORTES GENERALES J&amp;F S.A.C</t>
-        </is>
-      </c>
-      <c r="D79" t="n">
-        <v>6500</v>
-      </c>
-      <c r="E79" t="n">
-        <v>4</v>
-      </c>
-      <c r="F79" t="n">
-        <v>1</v>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>P266</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>SANTIAGO DE SURCO</t>
-        </is>
-      </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>E/S MONTREAL</t>
-        </is>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Av. Caminos del Inca 2017, Santiago de Surco 15039</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>ANC-872</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>TRANSPORTES GENERALES J&amp;F S.A.C</t>
-        </is>
-      </c>
-      <c r="D80" t="n">
-        <v>6500</v>
-      </c>
-      <c r="E80" t="n">
-        <v>4</v>
-      </c>
-      <c r="F80" t="n">
-        <v>2</v>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>P218</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>CALLAO</t>
-        </is>
-      </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>E/S ESCOSA</t>
-        </is>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>Av. Guardia Civil Sur 341, Chorrillos 15056</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>ANC-872</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>TRANSPORTES GENERALES J&amp;F S.A.C</t>
-        </is>
-      </c>
-      <c r="D81" t="n">
-        <v>6500</v>
-      </c>
-      <c r="E81" t="n">
-        <v>4</v>
-      </c>
-      <c r="F81" t="n">
-        <v>3</v>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>P167</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>MIRAFLORES</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>E/S MIRAFLORES</t>
-        </is>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>VXGG+H2W, Lima 15074</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>ANC-872</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>TRANSPORTES GENERALES J&amp;F S.A.C</t>
-        </is>
-      </c>
-      <c r="D82" t="n">
-        <v>6500</v>
-      </c>
-      <c r="E82" t="n">
-        <v>4</v>
-      </c>
-      <c r="F82" t="n">
-        <v>4</v>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>P327</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>ZARATE</t>
-        </is>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>E/S ZARATE</t>
-        </is>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Av. Malecón Checa, San Juan de Lurigancho 15401</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>B7N-933</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>INVERSIONES GALVEZ MARTINEZ</t>
-        </is>
-      </c>
-      <c r="D83" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E83" t="n">
-        <v>7</v>
-      </c>
-      <c r="F83" t="n">
-        <v>1</v>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>P193</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>CHILCA</t>
-        </is>
-      </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>E/S CHILCA</t>
-        </is>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>1S, Chilca 15871</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>B7N-933</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>INVERSIONES GALVEZ MARTINEZ</t>
-        </is>
-      </c>
-      <c r="D84" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E84" t="n">
-        <v>7</v>
-      </c>
-      <c r="F84" t="n">
-        <v>2</v>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>P246</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>SAN MIGUEL</t>
-        </is>
-      </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>E/S LA PAZ 1</t>
-        </is>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Av. La Paz 925, San Miguel 15087</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>B7N-933</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>INVERSIONES GALVEZ MARTINEZ</t>
-        </is>
-      </c>
-      <c r="D85" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E85" t="n">
-        <v>7</v>
-      </c>
-      <c r="F85" t="n">
-        <v>3</v>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>P327</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>ZARATE</t>
-        </is>
-      </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>E/S ZARATE</t>
-        </is>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Av. Malecón Checa, San Juan de Lurigancho 15401</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="n">
-        <v>84</v>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>AHJ-851</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D86" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E86" t="n">
-        <v>6</v>
-      </c>
-      <c r="F86" t="n">
-        <v>1</v>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>P193</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>CHILCA</t>
-        </is>
-      </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>E/S CHILCA</t>
-        </is>
-      </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>1S, Chilca 15871</t>
-        </is>
-      </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>AHJ-851</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D87" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E87" t="n">
-        <v>6</v>
-      </c>
-      <c r="F87" t="n">
-        <v>2</v>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>P316</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>CHORRILLOS</t>
-        </is>
-      </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>E/S TAVIRSA</t>
-        </is>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>Av. Prol. Huaylas 600, Lima 15067</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="1" t="n">
-        <v>86</v>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>AHJ-851</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D88" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E88" t="n">
-        <v>6</v>
-      </c>
-      <c r="F88" t="n">
-        <v>3</v>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>P246</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>SAN MIGUEL</t>
-        </is>
-      </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>E/S LA PAZ 1</t>
-        </is>
-      </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>Av. La Paz 925, San Miguel 15087</t>
-        </is>
-      </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>F2F-729</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D89" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E89" t="n">
-        <v>7</v>
-      </c>
-      <c r="F89" t="n">
-        <v>1</v>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>P316</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>CHORRILLOS</t>
-        </is>
-      </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>E/S TAVIRSA</t>
-        </is>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>Av. Prol. Huaylas 600, Lima 15067</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>F2F-729</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D90" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E90" t="n">
-        <v>7</v>
-      </c>
-      <c r="F90" t="n">
-        <v>2</v>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>P246</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>SAN MIGUEL</t>
-        </is>
-      </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>E/S LA PAZ 1</t>
-        </is>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>Av. La Paz 925, San Miguel 15087</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>F2F-729</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D91" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E91" t="n">
-        <v>7</v>
-      </c>
-      <c r="F91" t="n">
-        <v>3</v>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>P353</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>SAN ISIDRO</t>
-        </is>
-      </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>E/S MARBELLA</t>
-        </is>
-      </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>Av. Augusto Pérez Araníbar 2199, San Isidro 15076</t>
-        </is>
-      </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>F2F-729</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>TRANSLYM</t>
-        </is>
-      </c>
-      <c r="D92" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E92" t="n">
-        <v>7</v>
-      </c>
-      <c r="F92" t="n">
-        <v>4</v>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>P110</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>PUENTE PIEDRA</t>
-        </is>
-      </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>E/S NEOX</t>
-        </is>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>Leoncio Prado 888, Puente Piedra 15122</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>BCQ-737</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>MULTITRANS RR</t>
-        </is>
-      </c>
-      <c r="D93" t="n">
-        <v>4500</v>
-      </c>
-      <c r="E93" t="n">
-        <v>6</v>
-      </c>
-      <c r="F93" t="n">
-        <v>1</v>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>P353</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>SAN ISIDRO</t>
-        </is>
-      </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>E/S MARBELLA</t>
-        </is>
-      </c>
-      <c r="J93" t="inlineStr">
-        <is>
-          <t>Av. Augusto Pérez Araníbar 2199, San Isidro 15076</t>
-        </is>
-      </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>BCQ-737</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>MULTITRANS RR</t>
-        </is>
-      </c>
-      <c r="D94" t="n">
-        <v>4500</v>
-      </c>
-      <c r="E94" t="n">
-        <v>6</v>
-      </c>
-      <c r="F94" t="n">
-        <v>2</v>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>P110</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>PUENTE PIEDRA</t>
-        </is>
-      </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>E/S NEOX</t>
-        </is>
-      </c>
-      <c r="J94" t="inlineStr">
-        <is>
-          <t>Leoncio Prado 888, Puente Piedra 15122</t>
-        </is>
-      </c>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>BCQ-737</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>MULTITRANS RR</t>
-        </is>
-      </c>
-      <c r="D95" t="n">
-        <v>4500</v>
-      </c>
-      <c r="E95" t="n">
-        <v>6</v>
-      </c>
-      <c r="F95" t="n">
-        <v>3</v>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>P260</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>PUENTE PIEDRA</t>
-        </is>
-      </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>E/S MEJIA</t>
-        </is>
-      </c>
-      <c r="J95" t="inlineStr">
-        <is>
-          <t>5V8P+7HQ, Puente Piedra 07076</t>
-        </is>
-      </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>BJV-928</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>MULTITRANS RR</t>
-        </is>
-      </c>
-      <c r="D96" t="n">
-        <v>4500</v>
-      </c>
-      <c r="E96" t="n">
-        <v>7</v>
-      </c>
-      <c r="F96" t="n">
-        <v>1</v>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>P260</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>PUENTE PIEDRA</t>
-        </is>
-      </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>E/S MEJIA</t>
-        </is>
-      </c>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>5V8P+7HQ, Puente Piedra 07076</t>
-        </is>
-      </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>COESTI</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>